<commit_message>
update some API info
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>API Name</t>
   </si>
@@ -126,13 +126,22 @@
   </si>
   <si>
     <t>1-ch image</t>
+  </si>
+  <si>
+    <t>cudaGammaCorrection</t>
+  </si>
+  <si>
+    <t>cudaAntisotropy</t>
+  </si>
+  <si>
+    <t>3-ch image, loop times is 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +152,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,18 +191,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -467,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +530,7 @@
       <c r="D2">
         <v>0.96699999999999997</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -521,7 +542,7 @@
       <c r="D3">
         <v>3.9</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -533,7 +554,7 @@
       <c r="D4">
         <v>0.92100000000000004</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -545,7 +566,7 @@
       <c r="D5">
         <v>3.71</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -557,7 +578,7 @@
       <c r="D6">
         <v>0.21299999999999999</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -569,7 +590,7 @@
       <c r="D7">
         <v>0.85</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -581,7 +602,7 @@
       <c r="D8">
         <v>0.47199999999999998</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -593,7 +614,7 @@
       <c r="D9">
         <v>1.85</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -605,7 +626,7 @@
       <c r="D10">
         <v>1.4239999999999999</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -617,7 +638,7 @@
       <c r="D11">
         <v>5.67</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -629,7 +650,7 @@
       <c r="D12">
         <v>0.56299999999999994</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -641,7 +662,7 @@
       <c r="D13">
         <v>2.21</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -653,7 +674,7 @@
       <c r="D14">
         <v>0.58499999999999996</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -665,7 +686,7 @@
       <c r="D15">
         <v>2.2200000000000002</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -677,7 +698,7 @@
       <c r="D16">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -689,7 +710,7 @@
       <c r="D17">
         <v>0.89300000000000002</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -837,29 +858,66 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>0.876</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>3.492</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6">
+        <v>16.277000000000001</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6">
+        <v>65.289000000000001</v>
+      </c>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="E28:E29"/>
+  <mergeCells count="33">
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="E32:E33"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="A4:A5"/>
@@ -874,7 +932,25 @@
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>